<commit_message>
evaluation, fixes and tex
</commit_message>
<xml_diff>
--- a/10/evaluation.xlsx
+++ b/10/evaluation.xlsx
@@ -848,7 +848,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Anzahl Nachrichten auf Ring (n = 10000)</a:t>
+              <a:t>Anzahl Nachrichten auf Ring (n = 10000) Version 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1541,6 +1541,734 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Anzahl Nachrichten auf Ring (n = 10000) Version 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-AT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AA$5:$AA$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>184716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>212075</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>191554</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>189139</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>182530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>184959</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192988</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>186450</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>192228</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>184668</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196897</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>186752</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>187770</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>197244</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>174173</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>183607</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>208149</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>190137</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>189812</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>175608</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>181186</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>186850</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>198415</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>181828</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185352</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>190395</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>191848</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200280</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>183494</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>184807</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>182853</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>189519</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>187297</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>189558</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>189317</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>177819</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>182380</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>188857</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>175693</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>197255</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>189341</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>191928</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>190707</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>195659</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>197063</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>181471</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>182912</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>185272</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>189817</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>184355</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>180838</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>197431</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>184368</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>179683</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>193907</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>190744</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>180939</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>190115</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>194408</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>184281</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>185738</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>185219</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>180628</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>183530</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>178331</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>198880</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>189299</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>188256</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>184731</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>185856</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>179682</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>189096</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>185240</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>180981</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>173818</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>188587</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>188425</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>182733</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>181663</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>181080</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>196966</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>180601</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>203911</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>178233</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>191383</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>178352</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>183165</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>180576</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>187355</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>186892</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>196707</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>181019</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>187468</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>181883</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>179408</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>183616</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>178288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C92-41A5-9F29-D644F4176EEF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1892700168"/>
+        <c:axId val="1892701960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1892700168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Durchlauf</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-AT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1892701960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1892701960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Anzahl Nachrichten</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-AT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1892700168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-AT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1621,6 +2349,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2125,6 +2893,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2712,6 +3996,45 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85DF12C2-C004-4512-B189-D857ED93B9E1}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{BEF775AF-1336-491F-8B6B-52F04D82772B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3007,10 +4330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:X181"/>
+  <dimension ref="D4:AA181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,7 +4341,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>576172</v>
       </c>
@@ -3026,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>567308</v>
       </c>
@@ -3036,794 +4359,1094 @@
       <c r="X5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA5" s="1">
+        <v>184716</v>
+      </c>
+    </row>
+    <row r="6" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <v>550700</v>
       </c>
       <c r="W6" s="1">
         <v>97993</v>
       </c>
-    </row>
-    <row r="7" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA6" s="1">
+        <v>197663</v>
+      </c>
+    </row>
+    <row r="7" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <v>578572</v>
       </c>
       <c r="W7" s="1">
         <v>102541</v>
       </c>
-    </row>
-    <row r="8" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA7" s="1">
+        <v>212075</v>
+      </c>
+    </row>
+    <row r="8" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <v>546924</v>
       </c>
       <c r="W8" s="1">
         <v>90066</v>
       </c>
-    </row>
-    <row r="9" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA8" s="1">
+        <v>191554</v>
+      </c>
+    </row>
+    <row r="9" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>596708</v>
       </c>
       <c r="W9" s="1">
         <v>92984</v>
       </c>
-    </row>
-    <row r="10" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA9" s="1">
+        <v>180775</v>
+      </c>
+    </row>
+    <row r="10" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>569444</v>
       </c>
       <c r="W10" s="1">
         <v>93319</v>
       </c>
-    </row>
-    <row r="11" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA10" s="1">
+        <v>189139</v>
+      </c>
+    </row>
+    <row r="11" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>563492</v>
       </c>
       <c r="W11" s="1">
         <v>100883</v>
       </c>
-    </row>
-    <row r="12" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA11" s="1">
+        <v>182530</v>
+      </c>
+    </row>
+    <row r="12" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>576580</v>
       </c>
       <c r="W12" s="1">
         <v>92035</v>
       </c>
-    </row>
-    <row r="13" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA12" s="1">
+        <v>184959</v>
+      </c>
+    </row>
+    <row r="13" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>553220</v>
       </c>
       <c r="W13" s="1">
         <v>111864</v>
       </c>
-    </row>
-    <row r="14" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA13" s="1">
+        <v>192988</v>
+      </c>
+    </row>
+    <row r="14" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>556884</v>
       </c>
       <c r="W14" s="1">
         <v>89533</v>
       </c>
-    </row>
-    <row r="15" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA14" s="1">
+        <v>186450</v>
+      </c>
+    </row>
+    <row r="15" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>559260</v>
       </c>
       <c r="W15" s="1">
         <v>104469</v>
       </c>
-    </row>
-    <row r="16" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AA15" s="1">
+        <v>192228</v>
+      </c>
+    </row>
+    <row r="16" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>578556</v>
       </c>
       <c r="W16" s="1">
         <v>98185</v>
       </c>
-    </row>
-    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA16" s="1">
+        <v>180024</v>
+      </c>
+    </row>
+    <row r="17" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>574028</v>
       </c>
       <c r="W17" s="1">
         <v>105378</v>
       </c>
-    </row>
-    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA17" s="1">
+        <v>184668</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>591564</v>
       </c>
       <c r="W18" s="1">
         <v>93062</v>
       </c>
-    </row>
-    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA18" s="1">
+        <v>196897</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>582540</v>
       </c>
       <c r="W19" s="1">
         <v>95777</v>
       </c>
-    </row>
-    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA19" s="1">
+        <v>186752</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>565396</v>
       </c>
       <c r="W20" s="1">
         <v>96565</v>
       </c>
-    </row>
-    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA20" s="1">
+        <v>187770</v>
+      </c>
+    </row>
+    <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>562044</v>
       </c>
       <c r="W21" s="1">
         <v>98664</v>
       </c>
-    </row>
-    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA21" s="1">
+        <v>197244</v>
+      </c>
+    </row>
+    <row r="22" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>602572</v>
       </c>
       <c r="W22" s="1">
         <v>93649</v>
       </c>
-    </row>
-    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA22" s="1">
+        <v>174173</v>
+      </c>
+    </row>
+    <row r="23" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>566500</v>
       </c>
       <c r="W23" s="1">
         <v>104968</v>
       </c>
-    </row>
-    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA23" s="1">
+        <v>183607</v>
+      </c>
+    </row>
+    <row r="24" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>547780</v>
       </c>
       <c r="W24" s="1">
         <v>93391</v>
       </c>
-    </row>
-    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA24" s="1">
+        <v>208149</v>
+      </c>
+    </row>
+    <row r="25" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>546724</v>
       </c>
       <c r="W25" s="1">
         <v>104885</v>
       </c>
-    </row>
-    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA25" s="1">
+        <v>190137</v>
+      </c>
+    </row>
+    <row r="26" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>583644</v>
       </c>
       <c r="W26" s="1">
         <v>93455</v>
       </c>
-    </row>
-    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA26" s="1">
+        <v>189812</v>
+      </c>
+    </row>
+    <row r="27" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>572396</v>
       </c>
       <c r="W27" s="1">
         <v>101255</v>
       </c>
-    </row>
-    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA27" s="1">
+        <v>175608</v>
+      </c>
+    </row>
+    <row r="28" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>596148</v>
       </c>
       <c r="W28" s="1">
         <v>95794</v>
       </c>
-    </row>
-    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA28" s="1">
+        <v>181186</v>
+      </c>
+    </row>
+    <row r="29" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>558700</v>
       </c>
       <c r="W29" s="1">
         <v>92226</v>
       </c>
-    </row>
-    <row r="30" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA29" s="1">
+        <v>186850</v>
+      </c>
+    </row>
+    <row r="30" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <v>551308</v>
       </c>
       <c r="W30" s="1">
         <v>97588</v>
       </c>
-    </row>
-    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA30" s="1">
+        <v>198415</v>
+      </c>
+    </row>
+    <row r="31" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>581188</v>
       </c>
       <c r="W31" s="1">
         <v>99774</v>
       </c>
-    </row>
-    <row r="32" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA31" s="1">
+        <v>181828</v>
+      </c>
+    </row>
+    <row r="32" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>584924</v>
       </c>
       <c r="W32" s="1">
         <v>98412</v>
       </c>
-    </row>
-    <row r="33" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA32" s="1">
+        <v>185352</v>
+      </c>
+    </row>
+    <row r="33" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
         <v>592356</v>
       </c>
       <c r="W33" s="1">
         <v>101785</v>
       </c>
-    </row>
-    <row r="34" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA33" s="1">
+        <v>190395</v>
+      </c>
+    </row>
+    <row r="34" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <v>559108</v>
       </c>
       <c r="W34" s="1">
         <v>93674</v>
       </c>
-    </row>
-    <row r="35" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA34" s="1">
+        <v>191848</v>
+      </c>
+    </row>
+    <row r="35" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>589292</v>
       </c>
       <c r="W35" s="1">
         <v>93535</v>
       </c>
-    </row>
-    <row r="36" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA35" s="1">
+        <v>200280</v>
+      </c>
+    </row>
+    <row r="36" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>535036</v>
       </c>
       <c r="W36" s="1">
         <v>109234</v>
       </c>
-    </row>
-    <row r="37" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA36" s="1">
+        <v>183494</v>
+      </c>
+    </row>
+    <row r="37" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>583124</v>
       </c>
       <c r="W37" s="1">
         <v>84954</v>
       </c>
-    </row>
-    <row r="38" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA37" s="1">
+        <v>184807</v>
+      </c>
+    </row>
+    <row r="38" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D38" s="1">
         <v>565516</v>
       </c>
       <c r="W38" s="1">
         <v>97302</v>
       </c>
-    </row>
-    <row r="39" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA38" s="1">
+        <v>182853</v>
+      </c>
+    </row>
+    <row r="39" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D39" s="1">
         <v>576852</v>
       </c>
       <c r="W39" s="1">
         <v>108421</v>
       </c>
-    </row>
-    <row r="40" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA39" s="1">
+        <v>189519</v>
+      </c>
+    </row>
+    <row r="40" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
         <v>602212</v>
       </c>
       <c r="W40" s="1">
         <v>97954</v>
       </c>
-    </row>
-    <row r="41" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA40" s="1">
+        <v>187297</v>
+      </c>
+    </row>
+    <row r="41" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D41" s="1">
         <v>590692</v>
       </c>
       <c r="W41" s="1">
         <v>98835</v>
       </c>
-    </row>
-    <row r="42" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA41" s="1">
+        <v>189558</v>
+      </c>
+    </row>
+    <row r="42" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D42" s="1">
         <v>589476</v>
       </c>
       <c r="W42" s="1">
         <v>100230</v>
       </c>
-    </row>
-    <row r="43" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA42" s="1">
+        <v>189317</v>
+      </c>
+    </row>
+    <row r="43" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D43" s="1">
         <v>565220</v>
       </c>
       <c r="W43" s="1">
         <v>93182</v>
       </c>
-    </row>
-    <row r="44" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA43" s="1">
+        <v>177819</v>
+      </c>
+    </row>
+    <row r="44" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>532084</v>
       </c>
       <c r="W44" s="1">
         <v>91435</v>
       </c>
-    </row>
-    <row r="45" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA44" s="1">
+        <v>182380</v>
+      </c>
+    </row>
+    <row r="45" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D45" s="1">
         <v>561268</v>
       </c>
       <c r="W45" s="1">
         <v>101829</v>
       </c>
-    </row>
-    <row r="46" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA45" s="1">
+        <v>188857</v>
+      </c>
+    </row>
+    <row r="46" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D46" s="1">
         <v>542924</v>
       </c>
       <c r="W46" s="1">
         <v>103736</v>
       </c>
-    </row>
-    <row r="47" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA46" s="1">
+        <v>175693</v>
+      </c>
+    </row>
+    <row r="47" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D47" s="1">
         <v>570268</v>
       </c>
       <c r="W47" s="1">
         <v>99438</v>
       </c>
-    </row>
-    <row r="48" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA47" s="1">
+        <v>197255</v>
+      </c>
+    </row>
+    <row r="48" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D48" s="1">
         <v>573404</v>
       </c>
       <c r="W48" s="1">
         <v>91488</v>
       </c>
-    </row>
-    <row r="49" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA48" s="1">
+        <v>189341</v>
+      </c>
+    </row>
+    <row r="49" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D49" s="1">
         <v>561892</v>
       </c>
       <c r="W49" s="1">
         <v>95362</v>
       </c>
-    </row>
-    <row r="50" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA49" s="1">
+        <v>191928</v>
+      </c>
+    </row>
+    <row r="50" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D50" s="1">
         <v>601412</v>
       </c>
       <c r="W50" s="1">
         <v>102763</v>
       </c>
-    </row>
-    <row r="51" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA50" s="1">
+        <v>190707</v>
+      </c>
+    </row>
+    <row r="51" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D51" s="1">
         <v>588100</v>
       </c>
       <c r="W51" s="1">
         <v>98148</v>
       </c>
-    </row>
-    <row r="52" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA51" s="1">
+        <v>195659</v>
+      </c>
+    </row>
+    <row r="52" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D52" s="1">
         <v>602796</v>
       </c>
       <c r="W52" s="1">
         <v>93670</v>
       </c>
-    </row>
-    <row r="53" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA52" s="1">
+        <v>197063</v>
+      </c>
+    </row>
+    <row r="53" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D53" s="1">
         <v>572620</v>
       </c>
       <c r="W53" s="1">
         <v>90961</v>
       </c>
-    </row>
-    <row r="54" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA53" s="1">
+        <v>181471</v>
+      </c>
+    </row>
+    <row r="54" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D54" s="1">
         <v>581500</v>
       </c>
       <c r="W54" s="1">
         <v>104610</v>
       </c>
-    </row>
-    <row r="55" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA54" s="1">
+        <v>182912</v>
+      </c>
+    </row>
+    <row r="55" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D55" s="1">
         <v>568444</v>
       </c>
       <c r="W55" s="1">
         <v>101789</v>
       </c>
-    </row>
-    <row r="56" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA55" s="1">
+        <v>185272</v>
+      </c>
+    </row>
+    <row r="56" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D56" s="1">
         <v>592724</v>
       </c>
       <c r="W56" s="1">
         <v>99561</v>
       </c>
-    </row>
-    <row r="57" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA56" s="1">
+        <v>189817</v>
+      </c>
+    </row>
+    <row r="57" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D57" s="1">
         <v>577844</v>
       </c>
       <c r="W57" s="1">
         <v>92500</v>
       </c>
-    </row>
-    <row r="58" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA57" s="1">
+        <v>184355</v>
+      </c>
+    </row>
+    <row r="58" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D58" s="1">
         <v>561132</v>
       </c>
       <c r="W58" s="1">
         <v>98415</v>
       </c>
-    </row>
-    <row r="59" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA58" s="1">
+        <v>180838</v>
+      </c>
+    </row>
+    <row r="59" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D59" s="1">
         <v>562988</v>
       </c>
       <c r="W59" s="1">
         <v>99422</v>
       </c>
-    </row>
-    <row r="60" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA59" s="1">
+        <v>197431</v>
+      </c>
+    </row>
+    <row r="60" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D60" s="1">
         <v>567004</v>
       </c>
       <c r="W60" s="1">
         <v>98961</v>
       </c>
-    </row>
-    <row r="61" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA60" s="1">
+        <v>184368</v>
+      </c>
+    </row>
+    <row r="61" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D61" s="1">
         <v>553084</v>
       </c>
       <c r="W61" s="1">
         <v>99489</v>
       </c>
-    </row>
-    <row r="62" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA61" s="1">
+        <v>179683</v>
+      </c>
+    </row>
+    <row r="62" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D62" s="1">
         <v>546332</v>
       </c>
       <c r="W62" s="1">
         <v>101733</v>
       </c>
-    </row>
-    <row r="63" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA62" s="1">
+        <v>193907</v>
+      </c>
+    </row>
+    <row r="63" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D63" s="1">
         <v>552956</v>
       </c>
       <c r="W63" s="1">
         <v>92454</v>
       </c>
-    </row>
-    <row r="64" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA63" s="1">
+        <v>190744</v>
+      </c>
+    </row>
+    <row r="64" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D64" s="1">
         <v>597348</v>
       </c>
       <c r="W64" s="1">
         <v>93050</v>
       </c>
-    </row>
-    <row r="65" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA64" s="1">
+        <v>180939</v>
+      </c>
+    </row>
+    <row r="65" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D65" s="1">
         <v>586724</v>
       </c>
       <c r="W65" s="1">
         <v>104427</v>
       </c>
-    </row>
-    <row r="66" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA65" s="1">
+        <v>190115</v>
+      </c>
+    </row>
+    <row r="66" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D66" s="1">
         <v>613764</v>
       </c>
       <c r="W66" s="1">
         <v>91989</v>
       </c>
-    </row>
-    <row r="67" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA66" s="1">
+        <v>194408</v>
+      </c>
+    </row>
+    <row r="67" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D67" s="1">
         <v>564860</v>
       </c>
       <c r="W67" s="1">
         <v>97380</v>
       </c>
-    </row>
-    <row r="68" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA67" s="1">
+        <v>184281</v>
+      </c>
+    </row>
+    <row r="68" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D68" s="1">
         <v>564404</v>
       </c>
       <c r="W68" s="1">
         <v>92694</v>
       </c>
-    </row>
-    <row r="69" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA68" s="1">
+        <v>185738</v>
+      </c>
+    </row>
+    <row r="69" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D69" s="1">
         <v>573268</v>
       </c>
       <c r="W69" s="1">
         <v>92626</v>
       </c>
-    </row>
-    <row r="70" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA69" s="1">
+        <v>185219</v>
+      </c>
+    </row>
+    <row r="70" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D70" s="1">
         <v>593236</v>
       </c>
       <c r="W70" s="1">
         <v>89935</v>
       </c>
-    </row>
-    <row r="71" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA70" s="1">
+        <v>180628</v>
+      </c>
+    </row>
+    <row r="71" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D71" s="1">
         <v>565100</v>
       </c>
       <c r="W71" s="1">
         <v>102680</v>
       </c>
-    </row>
-    <row r="72" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA71" s="1">
+        <v>183530</v>
+      </c>
+    </row>
+    <row r="72" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D72" s="1">
         <v>573132</v>
       </c>
       <c r="W72" s="1">
         <v>100918</v>
       </c>
-    </row>
-    <row r="73" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA72" s="1">
+        <v>178331</v>
+      </c>
+    </row>
+    <row r="73" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D73" s="1">
         <v>596868</v>
       </c>
       <c r="W73" s="1">
         <v>102015</v>
       </c>
-    </row>
-    <row r="74" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA73" s="1">
+        <v>198880</v>
+      </c>
+    </row>
+    <row r="74" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D74" s="1">
         <v>557940</v>
       </c>
       <c r="W74" s="1">
         <v>101060</v>
       </c>
-    </row>
-    <row r="75" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA74" s="1">
+        <v>189299</v>
+      </c>
+    </row>
+    <row r="75" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D75" s="1">
         <v>596668</v>
       </c>
       <c r="W75" s="1">
         <v>90815</v>
       </c>
-    </row>
-    <row r="76" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA75" s="1">
+        <v>188256</v>
+      </c>
+    </row>
+    <row r="76" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D76" s="1">
         <v>590316</v>
       </c>
       <c r="W76" s="1">
         <v>95558</v>
       </c>
-    </row>
-    <row r="77" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA76" s="1">
+        <v>184731</v>
+      </c>
+    </row>
+    <row r="77" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D77" s="1">
         <v>591420</v>
       </c>
       <c r="W77" s="1">
         <v>97675</v>
       </c>
-    </row>
-    <row r="78" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA77" s="1">
+        <v>185856</v>
+      </c>
+    </row>
+    <row r="78" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D78" s="1">
         <v>565076</v>
       </c>
       <c r="W78" s="1">
         <v>91480</v>
       </c>
-    </row>
-    <row r="79" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA78" s="1">
+        <v>179682</v>
+      </c>
+    </row>
+    <row r="79" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D79" s="1">
         <v>540556</v>
       </c>
       <c r="W79" s="1">
         <v>94963</v>
       </c>
-    </row>
-    <row r="80" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA79" s="1">
+        <v>189096</v>
+      </c>
+    </row>
+    <row r="80" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D80" s="1">
         <v>540308</v>
       </c>
       <c r="W80" s="1">
         <v>98996</v>
       </c>
-    </row>
-    <row r="81" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA80" s="1">
+        <v>185240</v>
+      </c>
+    </row>
+    <row r="81" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D81" s="1">
         <v>567348</v>
       </c>
       <c r="W81" s="1">
         <v>106042</v>
       </c>
-    </row>
-    <row r="82" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA81" s="1">
+        <v>180981</v>
+      </c>
+    </row>
+    <row r="82" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D82" s="1">
         <v>573996</v>
       </c>
       <c r="W82" s="1">
         <v>96727</v>
       </c>
-    </row>
-    <row r="83" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA82" s="1">
+        <v>173818</v>
+      </c>
+    </row>
+    <row r="83" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D83" s="1">
         <v>572940</v>
       </c>
       <c r="W83" s="1">
         <v>107574</v>
       </c>
-    </row>
-    <row r="84" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA83" s="1">
+        <v>188587</v>
+      </c>
+    </row>
+    <row r="84" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D84" s="1">
         <v>550916</v>
       </c>
       <c r="W84" s="1">
         <v>97861</v>
       </c>
-    </row>
-    <row r="85" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA84" s="1">
+        <v>188425</v>
+      </c>
+    </row>
+    <row r="85" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D85" s="1">
         <v>584836</v>
       </c>
       <c r="W85" s="1">
         <v>85909</v>
       </c>
-    </row>
-    <row r="86" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA85" s="1">
+        <v>182733</v>
+      </c>
+    </row>
+    <row r="86" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D86" s="1">
         <v>557276</v>
       </c>
       <c r="W86" s="1">
         <v>96587</v>
       </c>
-    </row>
-    <row r="87" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA86" s="1">
+        <v>181663</v>
+      </c>
+    </row>
+    <row r="87" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D87" s="1">
         <v>553668</v>
       </c>
       <c r="W87" s="1">
         <v>101154</v>
       </c>
-    </row>
-    <row r="88" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA87" s="1">
+        <v>181080</v>
+      </c>
+    </row>
+    <row r="88" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D88" s="1">
         <v>578236</v>
       </c>
       <c r="W88" s="1">
         <v>95623</v>
       </c>
-    </row>
-    <row r="89" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA88" s="1">
+        <v>196966</v>
+      </c>
+    </row>
+    <row r="89" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D89" s="1">
         <v>581284</v>
       </c>
       <c r="W89" s="1">
         <v>90924</v>
       </c>
-    </row>
-    <row r="90" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA89" s="1">
+        <v>180601</v>
+      </c>
+    </row>
+    <row r="90" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D90" s="1">
         <v>551540</v>
       </c>
       <c r="W90" s="1">
         <v>97899</v>
       </c>
-    </row>
-    <row r="91" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA90" s="1">
+        <v>203911</v>
+      </c>
+    </row>
+    <row r="91" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D91" s="1">
         <v>568596</v>
       </c>
       <c r="W91" s="1">
         <v>90382</v>
       </c>
-    </row>
-    <row r="92" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA91" s="1">
+        <v>178233</v>
+      </c>
+    </row>
+    <row r="92" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D92" s="1">
         <v>604508</v>
       </c>
       <c r="W92" s="1">
         <v>99166</v>
       </c>
-    </row>
-    <row r="93" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA92" s="1">
+        <v>191383</v>
+      </c>
+    </row>
+    <row r="93" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D93" s="1">
         <v>537220</v>
       </c>
       <c r="W93" s="1">
         <v>91777</v>
       </c>
-    </row>
-    <row r="94" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA93" s="1">
+        <v>178352</v>
+      </c>
+    </row>
+    <row r="94" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D94" s="1">
         <v>601676</v>
       </c>
       <c r="W94" s="1">
         <v>93548</v>
       </c>
-    </row>
-    <row r="95" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA94" s="1">
+        <v>183165</v>
+      </c>
+    </row>
+    <row r="95" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D95" s="1">
         <v>582644</v>
       </c>
       <c r="W95" s="1">
         <v>96712</v>
       </c>
-    </row>
-    <row r="96" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA95" s="1">
+        <v>180576</v>
+      </c>
+    </row>
+    <row r="96" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D96" s="1">
         <v>550636</v>
       </c>
       <c r="W96" s="1">
         <v>98722</v>
       </c>
-    </row>
-    <row r="97" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA96" s="1">
+        <v>187355</v>
+      </c>
+    </row>
+    <row r="97" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D97" s="1">
         <v>573876</v>
       </c>
       <c r="W97" s="1">
         <v>96935</v>
       </c>
-    </row>
-    <row r="98" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA97" s="1">
+        <v>186892</v>
+      </c>
+    </row>
+    <row r="98" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D98" s="1">
         <v>586684</v>
       </c>
       <c r="W98" s="1">
         <v>95226</v>
       </c>
-    </row>
-    <row r="99" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA98" s="1">
+        <v>196707</v>
+      </c>
+    </row>
+    <row r="99" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D99" s="1">
         <v>549764</v>
       </c>
       <c r="W99" s="1">
         <v>96451</v>
       </c>
-    </row>
-    <row r="100" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA99" s="1">
+        <v>181019</v>
+      </c>
+    </row>
+    <row r="100" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D100" s="1">
         <v>573244</v>
       </c>
       <c r="W100" s="1">
         <v>86192</v>
       </c>
-    </row>
-    <row r="101" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA100" s="1">
+        <v>187468</v>
+      </c>
+    </row>
+    <row r="101" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D101" s="1">
         <v>563684</v>
       </c>
       <c r="W101" s="1">
         <v>90163</v>
       </c>
-    </row>
-    <row r="102" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA101" s="1">
+        <v>181883</v>
+      </c>
+    </row>
+    <row r="102" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D102" s="1">
         <v>563348</v>
       </c>
       <c r="W102" s="1">
         <v>107198</v>
       </c>
-    </row>
-    <row r="103" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA102" s="1">
+        <v>179408</v>
+      </c>
+    </row>
+    <row r="103" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D103" s="1">
         <v>548948</v>
       </c>
       <c r="W103" s="1">
         <v>89867</v>
       </c>
-    </row>
-    <row r="104" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="AA103" s="1">
+        <v>183616</v>
+      </c>
+    </row>
+    <row r="104" spans="4:27" x14ac:dyDescent="0.25">
       <c r="W104" s="1">
         <v>92296</v>
+      </c>
+      <c r="AA104" s="1">
+        <v>178288</v>
       </c>
     </row>
     <row r="181" spans="8:8" x14ac:dyDescent="0.25">

</xml_diff>